<commit_message>
Commit <ommiting frawework with db utils,testcases,flows>
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiran\IdeaProjects\mgnetoSoftwareTesting\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688C1B67-6D13-4408-A0FD-BF8CC9598498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15030" windowHeight="6540"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -47,13 +52,55 @@
   </si>
   <si>
     <t>delhi</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>kinnu@gmail.com</t>
+  </si>
+  <si>
+    <t>tirupati</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l@gmail.com</t>
+  </si>
+  <si>
+    <t>tirupatiswamy</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Harish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,7 +140,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -101,6 +148,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -108,13 +156,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -152,7 +208,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -186,6 +242,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -220,9 +277,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -395,16 +453,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="24.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,8 +475,14 @@
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -431,8 +495,14 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -444,36 +514,84 @@
       </c>
       <c r="D3" t="s">
         <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>1234567893</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1234567894</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="mailto:kiran@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" display="mailto:kiran@gmail.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{DFE0918E-E421-4BA0-B203-75ADDCCFE132}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{C6C3754F-90EE-40FF-93E5-D44C749FA0C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>